<commit_message>
Merged local branch and git verison
</commit_message>
<xml_diff>
--- a/datasets/image_samples.xlsx
+++ b/datasets/image_samples.xlsx
@@ -803,109 +803,109 @@
     <t>WunLu3R</t>
   </si>
   <si>
-    <t>/img/kMAdymP.jpg</t>
-  </si>
-  <si>
-    <t>/img/4JWIvgu.jpg</t>
-  </si>
-  <si>
-    <t>/img/m27r7ex.jpg</t>
-  </si>
-  <si>
-    <t>/img/Ag7qwqa.jpg</t>
-  </si>
-  <si>
-    <t>/img/dpHTQXQ.jpg</t>
-  </si>
-  <si>
-    <t>/img/nitmHp9.jpg</t>
-  </si>
-  <si>
-    <t>/img/QwjXL0R.jpg</t>
-  </si>
-  <si>
-    <t>/img/yshu6r3.jpg</t>
-  </si>
-  <si>
-    <t>/img/qSxg1na.jpg</t>
-  </si>
-  <si>
-    <t>/img/BMKcKqB.jpg</t>
-  </si>
-  <si>
-    <t>/img/APyO1l0.jpg</t>
-  </si>
-  <si>
-    <t>/img/zQxIdxn.jpg</t>
-  </si>
-  <si>
-    <t>/img/U80FxiX.jpg</t>
-  </si>
-  <si>
-    <t>/img/HzKmSgu.jpg</t>
-  </si>
-  <si>
-    <t>/img/vy1Y0IU.jpg</t>
-  </si>
-  <si>
-    <t>/img/pIMXYre.jpg</t>
-  </si>
-  <si>
-    <t>/img/wN0gL93.jpg</t>
-  </si>
-  <si>
-    <t>/img/Rtq9WU6.jpg</t>
-  </si>
-  <si>
-    <t>/img/g0Szusx.jpg</t>
-  </si>
-  <si>
-    <t>/img/a1jw1Rf.jpg</t>
-  </si>
-  <si>
-    <t>/img/vGwXbRj.jpg</t>
-  </si>
-  <si>
-    <t>/img/k2e4eo1.jpg</t>
-  </si>
-  <si>
-    <t>/img/g661XYa.jpg</t>
-  </si>
-  <si>
-    <t>/img/VOyCtG3.jpg</t>
-  </si>
-  <si>
-    <t>/img/bRmdtQw.jpg</t>
-  </si>
-  <si>
-    <t>/img/O5c9QUq.jpg</t>
-  </si>
-  <si>
-    <t>/img/nHB5aju.jpg</t>
-  </si>
-  <si>
-    <t>/img/zzb8mOY.jpg</t>
-  </si>
-  <si>
-    <t>/img/wuUqOIG.jpg</t>
-  </si>
-  <si>
-    <t>/img/m2LKEP8.jpg</t>
-  </si>
-  <si>
-    <t>/img/ttSsz9n.jpg</t>
-  </si>
-  <si>
-    <t>/img/jsuXIBU.jpg</t>
-  </si>
-  <si>
-    <t>/img/f5k9EvL.jpg</t>
-  </si>
-  <si>
-    <t>/img/sM6V9Fo.jpg</t>
-  </si>
-  <si>
-    <t>/img/WunLu3R.jpg</t>
+    <t>img/kMAdymP.jpg</t>
+  </si>
+  <si>
+    <t>img/4JWIvgu.jpg</t>
+  </si>
+  <si>
+    <t>img/m27r7ex.jpg</t>
+  </si>
+  <si>
+    <t>img/Ag7qwqa.jpg</t>
+  </si>
+  <si>
+    <t>img/dpHTQXQ.jpg</t>
+  </si>
+  <si>
+    <t>img/nitmHp9.jpg</t>
+  </si>
+  <si>
+    <t>img/QwjXL0R.jpg</t>
+  </si>
+  <si>
+    <t>img/yshu6r3.jpg</t>
+  </si>
+  <si>
+    <t>img/qSxg1na.jpg</t>
+  </si>
+  <si>
+    <t>img/BMKcKqB.jpg</t>
+  </si>
+  <si>
+    <t>img/APyO1l0.jpg</t>
+  </si>
+  <si>
+    <t>img/zQxIdxn.jpg</t>
+  </si>
+  <si>
+    <t>img/U80FxiX.jpg</t>
+  </si>
+  <si>
+    <t>img/HzKmSgu.jpg</t>
+  </si>
+  <si>
+    <t>img/vy1Y0IU.jpg</t>
+  </si>
+  <si>
+    <t>img/pIMXYre.jpg</t>
+  </si>
+  <si>
+    <t>img/wN0gL93.jpg</t>
+  </si>
+  <si>
+    <t>img/Rtq9WU6.jpg</t>
+  </si>
+  <si>
+    <t>img/g0Szusx.jpg</t>
+  </si>
+  <si>
+    <t>img/a1jw1Rf.jpg</t>
+  </si>
+  <si>
+    <t>img/vGwXbRj.jpg</t>
+  </si>
+  <si>
+    <t>img/k2e4eo1.jpg</t>
+  </si>
+  <si>
+    <t>img/g661XYa.jpg</t>
+  </si>
+  <si>
+    <t>img/VOyCtG3.jpg</t>
+  </si>
+  <si>
+    <t>img/bRmdtQw.jpg</t>
+  </si>
+  <si>
+    <t>img/O5c9QUq.jpg</t>
+  </si>
+  <si>
+    <t>img/nHB5aju.jpg</t>
+  </si>
+  <si>
+    <t>img/zzb8mOY.jpg</t>
+  </si>
+  <si>
+    <t>img/wuUqOIG.jpg</t>
+  </si>
+  <si>
+    <t>img/m2LKEP8.jpg</t>
+  </si>
+  <si>
+    <t>img/ttSsz9n.jpg</t>
+  </si>
+  <si>
+    <t>img/jsuXIBU.jpg</t>
+  </si>
+  <si>
+    <t>img/f5k9EvL.jpg</t>
+  </si>
+  <si>
+    <t>img/sM6V9Fo.jpg</t>
+  </si>
+  <si>
+    <t>img/WunLu3R.jpg</t>
   </si>
 </sst>
 </file>

</xml_diff>